<commit_message>
Doc:Se realiza la documentación del caso para implementacion de control de fechas el modulo Odoo del SIA nuevo http://sia.agrocampo.vip/modulo_odoo/Informes/index.php
</commit_message>
<xml_diff>
--- a/INF GEREN DEV ERIK/PORTOS 73/REPORTES/MIGRACION DE REPORTES ODOO.xlsx
+++ b/INF GEREN DEV ERIK/PORTOS 73/REPORTES/MIGRACION DE REPORTES ODOO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desarrollador2\Desktop\INF GEREN\PORTOS 73\REPORTE_GERENCIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desarrollador2\Desktop\REPO_AGROCAMPO\INF GEREN DEV ERIK\PORTOS 73\REPORTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774877E1-C505-4A15-BE5E-ADB4C4408CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E03E3C-0BBC-42E7-A2B8-7A821F782059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{C544AB1A-D7FE-4BF7-A1DA-13B49C65F04B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C544AB1A-D7FE-4BF7-A1DA-13B49C65F04B}"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTARIO REPORTES" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="59">
   <si>
     <t>GERENCIA</t>
   </si>
@@ -206,13 +206,19 @@
   </si>
   <si>
     <t xml:space="preserve">SUBGRUPO </t>
+  </si>
+  <si>
+    <t>CASO CREADO</t>
+  </si>
+  <si>
+    <t>NO VA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +235,14 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -286,7 +300,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -402,11 +416,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -457,6 +506,39 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -472,38 +554,41 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3AA185-93ED-4571-B0E3-143C7FDD92E7}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -852,28 +937,28 @@
     <col min="8" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-    </row>
-    <row r="2" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="33"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="4" t="s">
         <v>39</v>
       </c>
@@ -883,411 +968,461 @@
       <c r="G2" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="H2" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="25" t="s">
+      <c r="H3" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="24"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="23" t="s">
+      <c r="H4" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="H5" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-      <c r="B7" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="H6" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28"/>
+      <c r="C7" s="43"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+    </row>
+    <row r="9" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C10" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="9" t="s">
+      <c r="D10" s="42"/>
+      <c r="E10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C11" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="10" t="s">
+      <c r="D11" s="37"/>
+      <c r="E11" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+    </row>
+    <row r="13" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="31"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B14" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="23"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="23" t="s">
+      <c r="H14" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="7" t="s">
+      <c r="D16" s="21"/>
+      <c r="E16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F16" s="7">
         <v>1</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="23" t="s">
+      <c r="G16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="H17" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="23"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="21"/>
       <c r="E19" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="23"/>
+      <c r="H19" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="21"/>
       <c r="E20" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="23"/>
+      <c r="H20" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="21"/>
       <c r="E21" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="23"/>
+      <c r="H21" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="21"/>
       <c r="E22" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="7"/>
+      <c r="H22" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="7" t="s">
-        <v>40</v>
-      </c>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="7"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
+      <c r="B25" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="H25" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="7"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
+      <c r="B27" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="25" t="s">
+      <c r="H27" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="27"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="27"/>
+      <c r="B29" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C29" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D29" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="7">
+      <c r="E29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="7">
         <v>1</v>
       </c>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="12" t="s">
+      <c r="G29" s="7"/>
+      <c r="H29" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="27"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="25" t="s">
+      <c r="E30" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
+      <c r="B31" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-    </row>
-    <row r="32" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+    </row>
+    <row r="33" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="31"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B34" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C34" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F33" s="7">
-        <v>1</v>
-      </c>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="11"/>
+      <c r="D34" s="15"/>
       <c r="E34" s="7" t="s">
         <v>51</v>
       </c>
@@ -1295,12 +1430,15 @@
         <v>1</v>
       </c>
       <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
+      <c r="H34" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="27"/>
       <c r="B35" s="11"/>
       <c r="C35" s="16" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="7" t="s">
@@ -1310,12 +1448,15 @@
         <v>1</v>
       </c>
       <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
+      <c r="H35" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="27"/>
       <c r="B36" s="11"/>
       <c r="C36" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="7" t="s">
@@ -1325,81 +1466,94 @@
         <v>1</v>
       </c>
       <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
+      <c r="H36" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="27"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+      <c r="C37" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="D37" s="11"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="18" t="s">
+      <c r="E37" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="10">
+        <v>1</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="27"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="27"/>
+      <c r="B39" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C39" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="16" t="s">
+      <c r="D39" s="11"/>
+      <c r="E39" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="27"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="D40" s="11"/>
       <c r="E40" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" s="18" t="s">
+      <c r="H40" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="27"/>
+      <c r="B41" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="27"/>
+      <c r="B42" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C42" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F41" s="7">
-        <v>1</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="16" t="s">
-        <v>46</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="7" t="s">
@@ -1408,13 +1562,18 @@
       <c r="F42" s="7">
         <v>1</v>
       </c>
-      <c r="G42" s="7"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
-      <c r="B43" s="18"/>
+      <c r="G42" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="27"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="7" t="s">
@@ -1424,12 +1583,15 @@
         <v>1</v>
       </c>
       <c r="G43" s="7"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
-      <c r="B44" s="18"/>
+      <c r="H43" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="27"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="7" t="s">
@@ -1439,116 +1601,147 @@
         <v>1</v>
       </c>
       <c r="G44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
+      <c r="H44" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="27"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1</v>
+      </c>
       <c r="G45" s="7"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
-      <c r="B46" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="H45" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="27"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="29"/>
-      <c r="B47" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="27"/>
+      <c r="B47" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
       <c r="E47" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
+      <c r="H47" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="28"/>
+      <c r="B48" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="49" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D49" s="31" t="s">
+      <c r="H49" s="43"/>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D50" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="2">
-        <f>COUNTIF(E3:E47,"s")</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D50" s="31" t="s">
+      <c r="E50" s="2">
+        <f>COUNTIF(E3:E48,"s")</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D51" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="2">
-        <f>COUNTIF(E3:E47,"n")</f>
+      <c r="E51" s="2">
+        <f>COUNTIF(E3:E48,"n")</f>
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D51" s="31" t="s">
+    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D52" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="2">
-        <f>E49+E50</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="J53" s="2"/>
+      <c r="E52" s="2">
+        <f>E50+E51</f>
+        <v>33</v>
+      </c>
     </row>
     <row r="54" spans="4:10" x14ac:dyDescent="0.25">
       <c r="J54" s="2"/>
     </row>
+    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J55" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B18:B22"/>
+  <mergeCells count="40">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="A34:A48"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A14:A31"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A9:A11"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A13:A30"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A33:A47"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B19:B23"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G7">
     <cfRule type="expression" dxfId="1" priority="5">

</xml_diff>